<commit_message>
Change from MW_th to MW
</commit_message>
<xml_diff>
--- a/SeminarPaper/Model/input data/tech.xlsx
+++ b/SeminarPaper/Model/input data/tech.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Documents\GitHub\EnergyEconomics\SeminarPaper\Model\input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113564FF-ACCD-4A1F-BC27-850C688E54C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1511C5-238D-4866-B77E-C11BC182758D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_param_all_technologies" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
-  <si>
-    <t xml:space="preserve">Technology    	</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Type</t>
   </si>
@@ -31,45 +35,12 @@
     <t>eta</t>
   </si>
   <si>
-    <t xml:space="preserve">Lignite       	</t>
-  </si>
-  <si>
     <t>disp</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.39			</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coal          	</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.415			</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas (CCGT)    	</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.495			</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind onshore  	</t>
-  </si>
-  <si>
     <t>nondisp</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1				</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind offshore 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV ground     	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV roof       	</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -91,22 +62,49 @@
     <t>AnnuityTot[EUR/MWa]</t>
   </si>
   <si>
-    <t>MC[EUR/MWhTh]</t>
-  </si>
-  <si>
     <t>Lifetime[a]</t>
   </si>
   <si>
     <t>CarbonContent[t/MWhTh]</t>
   </si>
   <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>0.35</t>
-  </si>
-  <si>
-    <t>0.2</t>
+    <t>CO2Price[€/t]</t>
+  </si>
+  <si>
+    <t>FuelPrice[€/MWh_th]</t>
+  </si>
+  <si>
+    <t>MC[EUR/MWh]</t>
+  </si>
+  <si>
+    <t>CarbonContent[t/MWh]</t>
+  </si>
+  <si>
+    <t>FuelPrice[€/MWh]</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Lignite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal	</t>
+  </si>
+  <si>
+    <t>WindOnshore</t>
+  </si>
+  <si>
+    <t>WindOffshore</t>
+  </si>
+  <si>
+    <t>PVGround</t>
+  </si>
+  <si>
+    <t>PVRoof</t>
   </si>
 </sst>
 </file>
@@ -599,13 +597,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -961,71 +966,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="3">
         <v>1596</v>
@@ -1049,21 +1069,36 @@
         <v>139293.7285</v>
       </c>
       <c r="J2" s="3">
-        <v>20.43</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
+        <v>0.36</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K8" si="0">J2/P2</f>
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="L2" s="3">
+        <v>40</v>
+      </c>
+      <c r="M2" s="5">
+        <v>6.03</v>
+      </c>
+      <c r="N2">
+        <f>M2/P2</f>
+        <v>15.461538461538462</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" ref="O2:O8" si="1">(M2+(J2*L2))/(P2)</f>
+        <v>52.38461538461538</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
         <v>1957</v>
@@ -1087,21 +1122,36 @@
         <v>162104.21470000001</v>
       </c>
       <c r="J3" s="3">
-        <v>22.83</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
+        <v>0.35</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0.84337349397590355</v>
+      </c>
+      <c r="L3" s="3">
+        <v>40</v>
+      </c>
+      <c r="M3" s="5">
+        <v>8.83</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="2">M3/P3</f>
+        <v>21.277108433734941</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" si="1"/>
+        <v>55.012048192771083</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>928</v>
@@ -1125,21 +1175,36 @@
         <v>78710.889760000005</v>
       </c>
       <c r="J4" s="3">
-        <v>36.69</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
+        <v>0.2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0.40404040404040409</v>
+      </c>
+      <c r="L4" s="3">
+        <v>40</v>
+      </c>
+      <c r="M4" s="5">
+        <v>28.69</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>57.959595959595966</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="1"/>
+        <v>74.12121212121211</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>1548</v>
@@ -1165,19 +1230,34 @@
       <c r="J5" s="3">
         <v>0</v>
       </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>40</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3">
         <v>2473</v>
@@ -1203,19 +1283,34 @@
       <c r="J6" s="3">
         <v>0</v>
       </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>40</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
         <v>774</v>
@@ -1241,19 +1336,34 @@
       <c r="J7" s="3">
         <v>0</v>
       </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>40</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
         <v>972</v>
@@ -1279,37 +1389,72 @@
       <c r="J8" s="3">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>40</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>0.05</v>
       </c>
@@ -1337,5 +1482,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>